<commit_message>
ClueBoard Part 2 Done
</commit_message>
<xml_diff>
--- a/ClueLayout.xlsx
+++ b/ClueLayout.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="576" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="43">
   <si>
     <t>C</t>
   </si>
@@ -124,6 +124,27 @@
   </si>
   <si>
     <t>SL</t>
+  </si>
+  <si>
+    <t>Number of Doors : 14</t>
+  </si>
+  <si>
+    <t>White: Targets tests</t>
+  </si>
+  <si>
+    <t>Light Blue: walkway adjacency tests</t>
+  </si>
+  <si>
+    <t>Light Purple: adjacency tests, room exits</t>
+  </si>
+  <si>
+    <t>Dark Green: adjacency tests, beside room entrance</t>
+  </si>
+  <si>
+    <t>Orange: adjacency tests, inside rooms</t>
+  </si>
+  <si>
+    <t>All doors are tested for direction in ClueBoardTests</t>
   </si>
 </sst>
 </file>
@@ -188,12 +209,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="65"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
@@ -201,6 +216,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
@@ -221,29 +242,28 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="3"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="8"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="5"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" xfId="7"/>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="6"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="6" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="8"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="20% - Accent4" xfId="6" builtinId="42"/>
     <cellStyle name="40% - Accent3" xfId="3" builtinId="39"/>
-    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
-    <cellStyle name="60% - Accent6" xfId="8" builtinId="52"/>
+    <cellStyle name="60% - Accent4" xfId="6" builtinId="44"/>
+    <cellStyle name="60% - Accent5" xfId="8" builtinId="48"/>
+    <cellStyle name="60% - Accent6" xfId="7" builtinId="52"/>
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
     <cellStyle name="Accent2" xfId="2" builtinId="33"/>
     <cellStyle name="Accent3" xfId="5" builtinId="37"/>
@@ -547,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z25"/>
+  <dimension ref="A1:Z33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="AB9" sqref="AB9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -871,7 +891,7 @@
       <c r="D5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" t="s">
         <v>12</v>
       </c>
       <c r="F5" s="3" t="s">
@@ -963,7 +983,7 @@
       <c r="H6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="I6" t="s">
         <v>19</v>
       </c>
       <c r="J6" s="4" t="s">
@@ -1470,7 +1490,7 @@
       <c r="Q12" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="R12" s="1" t="s">
+      <c r="R12" t="s">
         <v>9</v>
       </c>
       <c r="S12" s="2" t="s">
@@ -1861,7 +1881,7 @@
       <c r="P17" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="Q17" s="3" t="s">
+      <c r="Q17" t="s">
         <v>12</v>
       </c>
       <c r="R17" s="3" t="s">
@@ -2127,7 +2147,7 @@
       <c r="F21" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="G21" s="3" t="s">
+      <c r="G21" t="s">
         <v>12</v>
       </c>
       <c r="H21" s="3" t="s">
@@ -2385,7 +2405,7 @@
       <c r="R24" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="S24" s="11" t="s">
+      <c r="S24" s="10" t="s">
         <v>12</v>
       </c>
       <c r="T24" s="2" t="s">
@@ -2473,6 +2493,41 @@
       </c>
       <c r="W25">
         <v>23</v>
+      </c>
+    </row>
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>